<commit_message>
Updated informations about languages
My resume improved with my language skills
</commit_message>
<xml_diff>
--- a/data/cv.xlsx
+++ b/data/cv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profils\mcanouil\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CEC2D70B-1E0F-43F8-822B-4FD85EAE9C66}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{92F5FD12-E321-4CE0-A5B0-22AB2D18315B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contact" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="91">
   <si>
     <t>position</t>
   </si>
@@ -118,9 +118,6 @@
     <t xml:space="preserve">C </t>
   </si>
   <si>
-    <t>Python</t>
-  </si>
-  <si>
     <t>Python (system, parallel computing, programming)</t>
   </si>
   <si>
@@ -167,6 +164,24 @@
   </si>
   <si>
     <t>Haskell</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>C1/C2 (native tongue)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English </t>
+  </si>
+  <si>
+    <t>B1/B2</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>A2/B1</t>
   </si>
   <si>
     <t>degree</t>
@@ -314,7 +329,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -329,6 +344,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -352,13 +374,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -733,16 +758,16 @@
         <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -766,7 +791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -835,10 +860,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -882,7 +907,7 @@
         <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -890,13 +915,13 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
         <v>20</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -904,13 +929,13 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
         <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -918,153 +943,195 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" t="s">
         <v>20</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" t="s">
-        <v>29</v>
-      </c>
       <c r="F7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" t="s">
         <v>28</v>
-      </c>
-      <c r="G7" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" t="s">
         <v>33</v>
-      </c>
-      <c r="F12" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
         <v>36</v>
       </c>
-      <c r="B14" t="s">
-        <v>37</v>
-      </c>
       <c r="F14" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" t="s">
         <v>36</v>
-      </c>
-      <c r="G14" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
         <v>39</v>
       </c>
-      <c r="F16" t="s">
-        <v>36</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" t="s">
         <v>39</v>
+      </c>
+      <c r="G17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1088,122 +1155,122 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
         <v>51</v>
       </c>
-      <c r="B3" t="s">
-        <v>46</v>
-      </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" t="s">
         <v>58</v>
       </c>
-      <c r="E4" t="s">
-        <v>53</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="E5" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" t="s">
         <v>66</v>
       </c>
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D6" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E6" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="F6" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1241,33 +1308,33 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="E2" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="F2" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1318,16 +1385,16 @@
         <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1356,25 +1423,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B1" t="s">
         <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="F1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="G1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1401,7 +1468,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1410,13 +1477,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1449,16 +1516,16 @@
         <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:5">

</xml_diff>

<commit_message>
Resume available in French and English
Resume done, maybe to improve later
</commit_message>
<xml_diff>
--- a/data/cv.xlsx
+++ b/data/cv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profils\mcanouil\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{92F5FD12-E321-4CE0-A5B0-22AB2D18315B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{184CFA8F-C750-4BC8-A511-EC1B2A6A1832}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contact" sheetId="1" r:id="rId1"/>
@@ -47,12 +47,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="104">
   <si>
     <t>position</t>
   </si>
   <si>
-    <t>institute</t>
+    <t>age</t>
   </si>
   <si>
     <t>city</t>
@@ -73,6 +73,9 @@
     <t>Student</t>
   </si>
   <si>
+    <t>28 years old</t>
+  </si>
+  <si>
     <t>Artres, France</t>
   </si>
   <si>
@@ -100,10 +103,7 @@
     <t>show</t>
   </si>
   <si>
-    <t>Curriculum Vitæ</t>
-  </si>
-  <si>
-    <t>I'm currently student, with an autistic trouble (asperger) and higher IQ, in M.S. in Bioinformatics and Computational Biology at the University of Lille (France). I'm looking for an internship about (epi)genectics  diseases. I'd recently discovered my troubles, and I'm learning to work with its to be better.</t>
+    <t>Looking for an internship on Bioinformatics or biological science computing in the medical field</t>
   </si>
   <si>
     <t>what</t>
@@ -261,7 +261,7 @@
   </si>
   <si>
     <t>Algorithms, complexity, databases
-After having been introduced to science computing research by Pr. Sylvain Salvati
+After having been introduced to science computing research by [Pr. Sylvain Salvati](sylvain.salvati@univ-lille.fr)
 And having achieved a research internship (70 hours) on "Solving Integro-Differential Equations and Neurobiology" with Dr. François Lemaire</t>
   </si>
   <si>
@@ -277,9 +277,30 @@
     <t>Expected graduation : Jul. 2021</t>
   </si>
   <si>
+    <t>institute</t>
+  </si>
+  <si>
     <t>activities</t>
   </si>
   <si>
+    <t>Volontary Tour Guide and Volontary Manager</t>
+  </si>
+  <si>
+    <t>["Club du Vieux Manoir"](https://www.clubduvieuxmanoir.fr/)</t>
+  </si>
+  <si>
+    <t>Chateau fort de Guise</t>
+  </si>
+  <si>
+    <t>Jul. 2008</t>
+  </si>
+  <si>
+    <t>Jul. 2017</t>
+  </si>
+  <si>
+    <t>Public reception, commented visits, mentoring young peope to restore historical monuments</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mathematics Teacher </t>
   </si>
   <si>
@@ -295,7 +316,25 @@
     <t>Aug. 2018</t>
   </si>
   <si>
-    <t>Management, teaching in secondary-school, collaboration</t>
+    <t>Management, teaching in secondary-school, collaboration, creation of informatics projects</t>
+  </si>
+  <si>
+    <t>Volunteer</t>
+  </si>
+  <si>
+    <t>["Institut Pasteur de Lille"](https://www.pasteur-lille.fr/accueil/)</t>
+  </si>
+  <si>
+    <t>Lille</t>
+  </si>
+  <si>
+    <t>Jan. 2020</t>
+  </si>
+  <si>
+    <t>Now</t>
+  </si>
+  <si>
+    <t>Public reception at the Institut Pasteur and/or its museum, group management, communication</t>
   </si>
   <si>
     <t>type</t>
@@ -670,7 +709,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -713,20 +752,23 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -755,19 +797,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="E1" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -791,41 +833,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="88.42578125" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
     <col min="3" max="3" width="67.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="75">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="C2" s="1"/>
       <c r="D2">
         <v>1</v>
       </c>
@@ -862,8 +902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -876,7 +916,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>19</v>
@@ -1143,13 +1183,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="57.85546875" customWidth="1"/>
+    <col min="2" max="2" width="38.140625" customWidth="1"/>
     <col min="6" max="6" width="142.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1173,7 +1214,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="27.75" customHeight="1">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -1285,13 +1326,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="50" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="117.42578125" bestFit="1" customWidth="1"/>
@@ -1302,7 +1345,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1314,37 +1357,68 @@
         <v>48</v>
       </c>
       <c r="F1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="B7" s="1"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30">
+      <c r="A4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
       <c r="B8" s="1"/>
@@ -1359,6 +1433,9 @@
       <c r="B11" s="1"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F5">
+    <sortCondition descending="1" ref="D2:D5"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1382,19 +1459,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="E1" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1423,25 +1500,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="D1" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="E1" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="F1" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="G1" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1468,22 +1545,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="E1" t="s">
         <v>49</v>
       </c>
       <c r="F1" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1513,19 +1590,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="E1" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:5">

</xml_diff>